<commit_message>
New Update! Added the new key guides on buttons(Thank Imp11) Reuse on Reactor
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7000"/>
+    <workbookView windowWidth="19200" windowHeight="6880"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -3899,7 +3899,7 @@
     <t>Bait your enemies</t>
   </si>
   <si>
-    <t>我丢，大奖</t>
+    <t>大奖</t>
   </si>
   <si>
     <t>杀害你的人会立刻报告</t>
@@ -6773,8 +6773,8 @@
   <sheetPr/>
   <dimension ref="A1:R1053"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
-      <selection activeCell="D566" sqref="D566:D568"/>
+    <sheetView tabSelected="1" topLeftCell="A686" workbookViewId="0">
+      <selection activeCell="D706" sqref="D706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
Update 3 Improve button guide I will start replacing the new language system on Wednesday
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -6773,8 +6773,8 @@
   <sheetPr/>
   <dimension ref="A1:R1053"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A686" workbookViewId="0">
-      <selection activeCell="D706" sqref="D706"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>